<commit_message>
Update Agile Reference Stories Spreadsheet.xlsx
</commit_message>
<xml_diff>
--- a/Requirements/Agile Reference Stories Spreadsheet.xlsx
+++ b/Requirements/Agile Reference Stories Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kansas-my.sharepoint.com/personal/m605m285_home_ku_edu/Documents/581 Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{731E2720-59A6-4EE3-9A4A-08695D4DA4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFC64B46-F5AF-480A-8F97-9049E58EE021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5260" yWindow="500" windowWidth="17080" windowHeight="16100" xr2:uid="{25715675-3E76-4C40-8856-19541E423838}"/>
   </bookViews>
@@ -59,13 +59,13 @@
     <t>EECS 665 Lab 8</t>
   </si>
   <si>
-    <t>"Developed several C++ programs that demonstrated various undefined behaviors (divide by zero, out-of-bounds list index) as well as a Makefile suite to demonstrate all of the</t>
+    <t>"Developed several C++ programs that demonstrated various undefined behaviors (divide by zero, out-of-bounds list index) as well as a Makefile suite."</t>
   </si>
   <si>
     <t>EECS 168   FA23 Lab 1</t>
   </si>
   <si>
-    <t>Excercise 0 create a github repositiory where youw ill comming the next 2 execises. Excercise 1: write a python program to print the output on your screen. Excercise 2: Create a progra that distplays your name, major, and hobbies.</t>
+    <t>"Wrote a python program to print output to the screen and wrote another to display your name, major, and hobbies. Pushed both files to Github."</t>
   </si>
   <si>
     <t>EECS 168 FA23 Lab 7</t>
@@ -77,13 +77,13 @@
     <t>EECS 658 Assignment 1</t>
   </si>
   <si>
-    <t>" Using common pyhton libraires like pandas, sklearn, numpy , scipy. Create a program that trains and evalutes a Naive Bayes classifier on the iris dataset using 2-fold cross validation and combines the results in a 150 sample test set. the outputs should be an overall accuracy, a confusion matrix, and the precision, recall and F1 scores for each flower type "</t>
+    <t>" Wrote a program using numpy, scipy, scikit-learn, and pandas libraries to train and evaluate a Naive Bayes classifier on the iris dataset using 2-fold cross validation and combine the results in a 150 sample test set. The outputs displayed overall accuracy, a confusion matrix, and the precision, recall and F1 scores for each flower type."</t>
   </si>
   <si>
     <t>EECS 210: Assignment 1</t>
   </si>
   <si>
-    <t>" create a program  that prints out a truth table showing the logical equivalences of Demorgan's First and Second law, First  and Second Associative law,  [(p ∨ q) ∧ (p → r) ∧ (q → r)] → r ≡ T, and p ↔ q ≡ (p → q) ∧ (q → p)."</t>
+    <t>"Wrote a program to print out a truth table showing the logical equivalences of Demorgan's First and Second law, First and Second Associative law,  [(p ∨ q) ∧ (p → r) ∧ (q → r)] → r ≡ T, and p ↔ q ≡ (p → q) ∧ (q → p)."</t>
   </si>
   <si>
     <t>EECS 268 Blob Lab</t>
@@ -101,19 +101,19 @@
     <t>EECS 268: Lab 1</t>
   </si>
   <si>
-    <t xml:space="preserve"> Write a program that reads information from a file and queries the user for information present within the file. There should be 6 options to choose from: Print all gamnes Highest gbbons to lowest, print all games from a year, Time for a Game? whihc ask the use to say how much time they have to play a game  and prits a list of all gapes that can be played in the time given, The people VS Dr. gibbons. prints a list of all games with a rating completely different thant what dr. gibbons gave them, print based on ranking, which obtains a rakin from the user and p[rints all games that have at least that gibbons rank. and Exit the program</t>
+    <t>"Wrote a  program that reads game data from a file and provides six interactive options: list games by rating, filter by year, suggest games by available playtime, compare user ratings with Dr. Gibbons’, filter by minimum rank, and exit the program."</t>
   </si>
   <si>
     <t>EECS 665 Project 3</t>
   </si>
   <si>
-    <t>"Modified a C++ program to create an abstract syntax tree (AST) as part of the compiler for a new programming language being created as part of the class, then used this AST to re-print the input program using its semantic elements"</t>
+    <t>"Modified a C++ program to create an abstract syntax tree (AST) as part of the compiler for a new programming language being created as part of the class, then used this AST to re-print the input program using its semantic elements."</t>
   </si>
   <si>
     <t>EECS 563: HW4</t>
   </si>
   <si>
-    <t>" Create 2 sets of python files that will act as a client/server pairs that will communicate over a network, one pair will communicate using TCP protocol while the other will communicate using UDP. The server and client should also preferably be ran in separate devices"</t>
+    <t>"Made 2 sets of Python files to act as a client/server pairs that will communicate over a network. One pair communicated using TCP protocol while the other communicated using UDP. The server and client were run using separate devices."</t>
   </si>
   <si>
     <t>EECS 565 Spring 25</t>
@@ -143,7 +143,7 @@
     <t>EECS 388 FA24 Final Project</t>
   </si>
   <si>
-    <t>"Developed a C program that uses a LiDAR sensor and motor to simulate an autonomous car. The LiDAR sensor was used to detect the distance from the nearest object and trigger the LED light to simulate moving, slowing down, and stopping. "</t>
+    <t>"Developed a C program that uses a LiDAR sensor and motor to simulate an autonomous car. The LiDAR sensor was used to detect the distance from the nearest object and trigger the LED light to simulate moving, slowing down, and stopping."</t>
   </si>
   <si>
     <t>EECS 678 Quash Project</t>
@@ -192,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -263,11 +263,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -285,9 +305,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -295,6 +312,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -633,28 +656,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5208EBB9-4566-DA4B-A252-9B50BC0C2FD4}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="2" width="21.125" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="49.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -672,7 +695,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="62.25" customHeight="1">
+    <row r="3" spans="1:4" ht="64.5" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -682,11 +705,11 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="82.5" customHeight="1">
+    <row r="4" spans="1:4" ht="60.75" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -710,11 +733,11 @@
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="115.5" customHeight="1">
+    <row r="6" spans="1:4" ht="99" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -724,7 +747,7 @@
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -756,7 +779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="61.5">
+    <row r="9" spans="1:4" ht="66.75" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -770,7 +793,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="169.5">
+    <row r="10" spans="1:4" ht="82.5" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -780,7 +803,7 @@
       <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -794,11 +817,11 @@
       <c r="C11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="85.5" customHeight="1">
+    <row r="12" spans="1:4" ht="75" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -808,7 +831,7 @@
       <c r="C12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>25</v>
       </c>
     </row>
@@ -868,7 +891,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="87" customHeight="1">
+    <row r="17" spans="1:4" ht="81.75" customHeight="1">
       <c r="A17" s="1">
         <v>16</v>
       </c>

</xml_diff>